<commit_message>
Mofificación al archivo excel
Se agrega comentario
</commit_message>
<xml_diff>
--- a/paq 2_06052021/Gerencia_TODOS_Cuadro_Control1 (1).xlsx
+++ b/paq 2_06052021/Gerencia_TODOS_Cuadro_Control1 (1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\UNI-GERENCIA\paq 2_06052021\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702FF74D-9051-4656-95BD-D09E4681452D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paq2" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Paq4" sheetId="3" r:id="rId3"/>
     <sheet name="Paq5" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="126">
   <si>
     <t>CURSO GERENCIA - PAQUETE 2 - CUADRO DE CONTROL</t>
   </si>
@@ -411,12 +412,15 @@
   </si>
   <si>
     <t>trabajando jorge</t>
+  </si>
+  <si>
+    <t>Este también para modificar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -996,11 +1000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1271,9 @@
       <c r="G13" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="25" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="55">
@@ -1551,31 +1557,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5:B6" r:id="rId3" display="http://localhost/www/Uni_Gerencia1/paq2/contents/resources/js/ug_diapo3/ug_diapo3.js"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17:B18" r:id="rId13" display="http://localhost/www/Uni_Gerencia1/paq2/contents/resources/js/ug_diapo7/ug_diapo7.js"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B21" r:id="rId16"/>
-    <hyperlink ref="B22" r:id="rId17"/>
-    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5:B6" r:id="rId3" display="http://localhost/www/Uni_Gerencia1/paq2/contents/resources/js/ug_diapo3/ug_diapo3.js" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17:B18" r:id="rId13" display="http://localhost/www/Uni_Gerencia1/paq2/contents/resources/js/ug_diapo7/ug_diapo7.js" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
@@ -2028,16 +2034,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B8:B9" r:id="rId2" display="http://localhost/www/Uni_Gerencia1/paq3/contents/tema2/UGPP1_4.html"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
-    <hyperlink ref="B13" r:id="rId6"/>
-    <hyperlink ref="B14" r:id="rId7"/>
-    <hyperlink ref="B15" r:id="rId8"/>
-    <hyperlink ref="B17" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B8:B9" r:id="rId2" display="http://localhost/www/Uni_Gerencia1/paq3/contents/tema2/UGPP1_4.html" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B16" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
@@ -2045,7 +2051,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2251,12 +2257,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
@@ -2264,7 +2270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2399,9 +2405,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>

</xml_diff>